<commit_message>
found best sigma value
</commit_message>
<xml_diff>
--- a/Sigmaval-Trial.xlsx
+++ b/Sigmaval-Trial.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Trialing sigma values for NRBF Neural Network</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Sigma Value</t>
+  </si>
+  <si>
+    <t>After 1000 iterations</t>
   </si>
 </sst>
 </file>
@@ -89,12 +92,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,34 +381,40 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -410,55 +422,116 @@
       <c r="A4">
         <v>0.1</v>
       </c>
+      <c r="B4">
+        <v>6.2429489670499999E-3</v>
+      </c>
+      <c r="C4">
+        <v>9.6351352725800005E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.2</v>
       </c>
+      <c r="B5">
+        <v>4.1801512728500002E-2</v>
+      </c>
+      <c r="C5">
+        <v>7.4611736047299995E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.3</v>
       </c>
+      <c r="B6">
+        <v>5.3880318463000003E-2</v>
+      </c>
+      <c r="C6">
+        <v>6.6737257643200001E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.4</v>
       </c>
+      <c r="B7">
+        <v>5.95791092407E-2</v>
+      </c>
+      <c r="C7">
+        <v>6.3005857981199995E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.5</v>
       </c>
+      <c r="B8">
+        <v>6.1386997914900002E-2</v>
+      </c>
+      <c r="C8">
+        <v>6.4432628574000006E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.6</v>
       </c>
+      <c r="B9">
+        <v>6.7766513496199998E-2</v>
+      </c>
+      <c r="C9">
+        <v>6.7184776853599998E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.7</v>
       </c>
+      <c r="B10">
+        <v>7.5172345111699998E-2</v>
+      </c>
+      <c r="C10">
+        <v>7.0208215091100007E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0.8</v>
       </c>
+      <c r="B11">
+        <v>7.8758799082899997E-2</v>
+      </c>
+      <c r="C11">
+        <v>7.0483929371899998E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.9</v>
       </c>
+      <c r="B12">
+        <v>8.10244640352E-2</v>
+      </c>
+      <c r="C12">
+        <v>6.9668914569299994E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
+      <c r="B13">
+        <v>8.1940640442599993E-2</v>
+      </c>
+      <c r="C13">
+        <v>6.9197265331600005E-2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>